<commit_message>
Merged changes to use calculator and notepad
</commit_message>
<xml_diff>
--- a/common/messages.xlsx
+++ b/common/messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billah\Source\Repos\windowsscrapern\Common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilb\sinter\windowsscrapern\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3192" windowWidth="28728" windowHeight="4488"/>
+    <workbookView xWindow="0" yWindow="3195" windowWidth="28725" windowHeight="4485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="128">
   <si>
     <t>Source</t>
   </si>
@@ -399,12 +399,21 @@
   </si>
   <si>
     <t>ignore</t>
+  </si>
+  <si>
+    <t>action_expand_and_select</t>
+  </si>
+  <si>
+    <t>Expand a menu and choose a item from it</t>
+  </si>
+  <si>
+    <t>queue of UI's</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -942,7 +951,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1177,6 +1186,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1538,34 +1550,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.53125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.796875" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.19921875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.46484375" style="6" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="14.19921875" style="6" customWidth="1"/>
     <col min="12" max="12" width="14" style="6" customWidth="1"/>
     <col min="13" max="14" width="13.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1578,30 +1590,30 @@
       <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-    </row>
-    <row r="2" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E2" s="81" t="s">
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+    </row>
+    <row r="2" spans="1:14" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
       <c r="M2" s="11" t="s">
         <v>11</v>
       </c>
@@ -1609,7 +1621,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1622,14 +1634,14 @@
       <c r="H3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="90"/>
-    </row>
-    <row r="4" spans="1:14" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="91"/>
+    </row>
+    <row r="4" spans="1:14" ht="13.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="I4" s="34" t="s">
         <v>17</v>
       </c>
@@ -1643,7 +1655,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1668,16 +1680,16 @@
       <c r="H5" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="88"/>
       <c r="M5" s="18"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1715,7 +1727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1740,14 +1752,14 @@
       <c r="H7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="84"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="87"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="88"/>
       <c r="M7" s="22"/>
       <c r="N7" s="15"/>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1785,7 +1797,7 @@
       </c>
       <c r="N8"/>
     </row>
-    <row r="9" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="24" t="s">
         <v>107</v>
       </c>
@@ -1817,7 +1829,7 @@
       </c>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="2"/>
@@ -1830,7 +1842,7 @@
       <c r="L10" s="65"/>
       <c r="M10" s="27"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1854,7 +1866,7 @@
       <c r="M11" s="16"/>
       <c r="N11" s="33"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1890,7 +1902,7 @@
       </c>
       <c r="N12" s="32"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1926,7 +1938,7 @@
       </c>
       <c r="N13" s="9"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1962,7 +1974,7 @@
       </c>
       <c r="N14" s="17"/>
     </row>
-    <row r="15" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="24" t="s">
         <v>116</v>
       </c>
@@ -1998,7 +2010,7 @@
       </c>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="28" t="s">
         <v>99</v>
       </c>
@@ -2032,7 +2044,7 @@
       </c>
       <c r="N16" s="30"/>
     </row>
-    <row r="17" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="24" t="s">
         <v>97</v>
       </c>
@@ -2064,7 +2076,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="28" t="s">
         <v>98</v>
       </c>
@@ -2098,7 +2110,7 @@
       </c>
       <c r="N18" s="77"/>
     </row>
-    <row r="19" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="24" t="s">
         <v>102</v>
       </c>
@@ -2134,7 +2146,7 @@
       </c>
       <c r="N19" s="57"/>
     </row>
-    <row r="20" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="24" t="s">
         <v>108</v>
       </c>
@@ -2170,11 +2182,11 @@
       </c>
       <c r="N20" s="57"/>
     </row>
-    <row r="21" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="28"/>
       <c r="B22" s="28"/>
       <c r="C22" s="23"/>
@@ -2190,7 +2202,7 @@
       <c r="M22" s="29"/>
       <c r="N22" s="29"/>
     </row>
-    <row r="23" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="28" t="s">
         <v>83</v>
       </c>
@@ -2224,7 +2236,7 @@
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
     </row>
-    <row r="24" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="28" t="s">
         <v>109</v>
       </c>
@@ -2258,11 +2270,11 @@
       <c r="M24" s="29"/>
       <c r="N24" s="29"/>
     </row>
-    <row r="25" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
@@ -2278,11 +2290,11 @@
       <c r="M26" s="73"/>
       <c r="N26" s="29"/>
     </row>
-    <row r="27" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -2317,7 +2329,7 @@
       <c r="L28" s="50"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="40" t="s">
         <v>39</v>
       </c>
@@ -2353,14 +2365,14 @@
       <c r="M29" s="30"/>
       <c r="N29" s="29"/>
     </row>
-    <row r="30" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="I30" s="6"/>
       <c r="K30" s="44"/>
       <c r="L30" s="44"/>
     </row>
-    <row r="31" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="39" t="s">
         <v>50</v>
       </c>
@@ -2377,7 +2389,7 @@
       <c r="K31" s="44"/>
       <c r="L31" s="44"/>
     </row>
-    <row r="32" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="24" t="s">
         <v>61</v>
       </c>
@@ -2415,7 +2427,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="28" t="s">
         <v>63</v>
       </c>
@@ -2455,7 +2467,7 @@
       <c r="M33" s="30"/>
       <c r="N33" s="29"/>
     </row>
-    <row r="34" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="24" t="s">
         <v>74</v>
       </c>
@@ -2495,7 +2507,7 @@
       <c r="M34" s="42"/>
       <c r="N34" s="29"/>
     </row>
-    <row r="35" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="24" t="s">
         <v>75</v>
       </c>
@@ -2533,7 +2545,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="28" t="s">
         <v>65</v>
       </c>
@@ -2573,7 +2585,7 @@
       <c r="M36" s="30"/>
       <c r="N36" s="29"/>
     </row>
-    <row r="37" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="28" t="s">
         <v>122</v>
       </c>
@@ -2601,11 +2613,11 @@
       <c r="M37" s="42"/>
       <c r="N37" s="29"/>
     </row>
-    <row r="38" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="24" t="s">
         <v>81</v>
       </c>
@@ -2627,7 +2639,7 @@
       <c r="M39"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -2661,7 +2673,7 @@
       <c r="M40" s="22"/>
       <c r="N40" s="15"/>
     </row>
-    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -2695,7 +2707,7 @@
       <c r="M41"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
@@ -2731,7 +2743,7 @@
       <c r="M42" s="22"/>
       <c r="N42" s="15"/>
     </row>
-    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -2765,7 +2777,7 @@
       <c r="K43" s="49"/>
       <c r="L43" s="27"/>
     </row>
-    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -2797,7 +2809,7 @@
       <c r="M44" s="22"/>
       <c r="N44" s="15"/>
     </row>
-    <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -2826,7 +2838,7 @@
       <c r="K45" s="50"/>
       <c r="L45" s="50"/>
     </row>
-    <row r="46" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
@@ -2849,14 +2861,14 @@
       <c r="H46" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I46" s="84"/>
-      <c r="J46" s="85"/>
+      <c r="I46" s="85"/>
+      <c r="J46" s="86"/>
       <c r="K46" s="33"/>
       <c r="L46" s="33"/>
       <c r="M46" s="22"/>
       <c r="N46" s="15"/>
     </row>
-    <row r="47" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2888,7 +2900,7 @@
       <c r="K47" s="50"/>
       <c r="L47" s="50"/>
     </row>
-    <row r="48" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="24" t="s">
         <v>120</v>
       </c>
@@ -2922,7 +2934,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A49" s="28" t="s">
         <v>117</v>
       </c>
@@ -2956,7 +2968,7 @@
       <c r="M49" s="22"/>
       <c r="N49" s="23"/>
     </row>
-    <row r="50" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A50" s="24" t="s">
         <v>118</v>
       </c>
@@ -2989,7 +3001,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" s="24" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A51" s="28" t="s">
         <v>121</v>
       </c>
@@ -3019,235 +3031,269 @@
       <c r="M51" s="22"/>
       <c r="N51" s="23"/>
     </row>
-    <row r="52" spans="1:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-    </row>
-    <row r="53" spans="1:14" s="24" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="39" t="s">
+    <row r="52" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="23">
+        <v>8</v>
+      </c>
+      <c r="F52" s="23">
+        <v>813</v>
+      </c>
+      <c r="G52" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52" s="79" t="s">
+        <v>127</v>
+      </c>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+      <c r="L52" s="79"/>
+      <c r="M52" s="79"/>
+      <c r="N52" s="23"/>
+    </row>
+    <row r="53" spans="1:14" ht="17.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="24"/>
+      <c r="B53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="84"/>
+      <c r="M53" s="24"/>
+      <c r="N53" s="24"/>
+    </row>
+    <row r="54" spans="1:14" s="24" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A54" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B54" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="2">
-        <v>9</v>
-      </c>
-      <c r="F53" s="2">
+      <c r="C54" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2">
+        <v>9</v>
+      </c>
+      <c r="F54" s="2">
         <v>900</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="6"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="71"/>
-    </row>
-    <row r="54" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="28" t="s">
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="6"/>
+      <c r="K54" s="71"/>
+      <c r="L54" s="71"/>
+    </row>
+    <row r="55" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A55" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B55" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="23">
-        <v>9</v>
-      </c>
-      <c r="F54" s="23">
+      <c r="C55" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="23">
+        <v>9</v>
+      </c>
+      <c r="F55" s="23">
         <v>901</v>
       </c>
-      <c r="G54" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I54" s="17" t="s">
+      <c r="G55" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I55" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J54" s="38" t="s">
+      <c r="J55" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="K54" s="37"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="29"/>
-    </row>
-    <row r="55" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="28" t="s">
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="29"/>
+    </row>
+    <row r="56" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A56" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B56" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" s="36">
-        <v>9</v>
-      </c>
-      <c r="F55" s="2">
+      <c r="C56" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="36">
+        <v>9</v>
+      </c>
+      <c r="F56" s="2">
         <v>902</v>
       </c>
-      <c r="G55" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H55" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I55" s="35" t="s">
+      <c r="G56" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I56" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="J55" s="35" t="s">
+      <c r="J56" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="K55" s="43"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="36"/>
-      <c r="N55" s="36"/>
-    </row>
-    <row r="56" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="K56" s="43"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="36"/>
+      <c r="N56" s="36"/>
+    </row>
+    <row r="57" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
         <v>114</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" s="2">
-        <v>9</v>
-      </c>
-      <c r="F56" s="2">
+      <c r="C57" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2">
+        <v>9</v>
+      </c>
+      <c r="F57" s="2">
         <v>903</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I56" s="17" t="s">
+      <c r="G57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I57" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="58" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
         <v>115</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="2">
-        <v>9</v>
-      </c>
-      <c r="F57" s="23">
+      <c r="C58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="2">
+        <v>9</v>
+      </c>
+      <c r="F58" s="23">
         <v>904</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I57" s="19" t="s">
+      <c r="G58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I58" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59" s="29" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A60" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="29" t="s">
+      <c r="B60" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C59" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="36">
+      <c r="C60" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="36">
         <v>10</v>
       </c>
-      <c r="F59" s="36">
+      <c r="F60" s="36">
         <v>1000</v>
       </c>
-      <c r="G59" s="29"/>
-      <c r="H59" s="29"/>
-      <c r="I59" s="29"/>
-      <c r="J59" s="29"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="29"/>
-      <c r="N59" s="29"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A60" s="24" t="s">
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="29"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A61" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B61" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" s="2">
+      <c r="C61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="2">
         <v>10</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F61" s="2">
         <v>1001</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J60" s="24"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
+      <c r="G61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="J61" s="24"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A62" s="24"/>
+      <c r="B62" s="24"/>
+      <c r="J62" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="E1:N1"/>
     <mergeCell ref="E2:L2"/>
-    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="K53:L53"/>
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="I3:L3"/>

</xml_diff>

<commit_message>
revise service_code/sub_code for verify_passcode messages
</commit_message>
<xml_diff>
--- a/common/messages.xlsx
+++ b/common/messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericafu/Documents/Github/sinter/common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3699587D-9692-4F49-B402-6AF31B947105}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1B68D2-E552-4E49-B4E0-030C80AB8213}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30500" yWindow="460" windowWidth="30520" windowHeight="21040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="460" windowWidth="30520" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="133">
   <si>
     <t>Source</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>verify_passcode</t>
+  </si>
+  <si>
+    <t>verify_passcode msgs between Server and Client</t>
   </si>
 </sst>
 </file>
@@ -508,7 +514,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +581,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -961,7 +973,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1231,6 +1243,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1558,13 +1579,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J66" sqref="J66"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3261,61 +3282,95 @@
       <c r="B61" s="24"/>
       <c r="J61" s="24"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" s="39" t="s">
+    <row r="62" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+    </row>
+    <row r="63" spans="1:14" s="91" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" s="92"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="93">
+        <v>99</v>
+      </c>
+      <c r="F63" s="93"/>
+      <c r="G63" s="93"/>
+      <c r="H63" s="93"/>
+      <c r="I63" s="92"/>
+      <c r="K63" s="92"/>
+      <c r="L63" s="92"/>
+      <c r="M63" s="93"/>
+      <c r="N63" s="93"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="B62" s="39" t="s">
+      <c r="B64" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="2">
+      <c r="C64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="2">
         <v>99</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F64" s="2">
         <v>9901</v>
       </c>
-      <c r="G62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H62" s="2" t="s">
+      <c r="G64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J64" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A63" s="39" t="s">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="39" t="s">
+      <c r="B65" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="2">
+      <c r="C65" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="2">
         <v>99</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F65" s="2">
         <v>9902</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H63" s="2" t="s">
+      <c r="G65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J65" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>